<commit_message>
finish proj3 pass all test
</commit_message>
<xml_diff>
--- a/docs/[61C SU22] Project 3B ROM Control Logic.xlsx
+++ b/docs/[61C SU22] Project 3B ROM Control Logic.xlsx
@@ -481,10 +481,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -573,9 +573,31 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -583,6 +605,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -596,16 +633,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -619,23 +700,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -651,74 +718,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -768,7 +768,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -780,13 +882,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -798,37 +936,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -840,115 +948,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -980,17 +980,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1036,29 +1041,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1080,148 +1080,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="34" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1580,11 +1580,11 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
+      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -3701,7 +3701,7 @@
         <v>26</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>98</v>
@@ -3726,15 +3726,15 @@
       </c>
       <c r="P31" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="Q31" s="31" t="str">
         <f t="shared" si="2"/>
-        <v>0001000001100101</v>
+        <v>0001000001100100</v>
       </c>
       <c r="R31" s="31" t="str">
         <f t="shared" si="3"/>
-        <v>01100101</v>
+        <v>01100100</v>
       </c>
       <c r="S31" s="31" t="str">
         <f t="shared" si="4"/>
@@ -3742,7 +3742,7 @@
       </c>
       <c r="T31" s="31" t="str">
         <f t="shared" ref="T31:U31" si="32">BIN2HEX(R31,2)</f>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U31" s="33" t="str">
         <f t="shared" si="32"/>
@@ -3773,7 +3773,7 @@
         <v>27</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>98</v>
@@ -3798,15 +3798,15 @@
       </c>
       <c r="P32" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="Q32" s="31" t="str">
         <f t="shared" si="2"/>
-        <v>0001000001100101</v>
+        <v>0001000001100100</v>
       </c>
       <c r="R32" s="31" t="str">
         <f t="shared" si="3"/>
-        <v>01100101</v>
+        <v>01100100</v>
       </c>
       <c r="S32" s="31" t="str">
         <f t="shared" si="4"/>
@@ -3814,7 +3814,7 @@
       </c>
       <c r="T32" s="31" t="str">
         <f t="shared" ref="T32:U32" si="33">BIN2HEX(R32,2)</f>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U32" s="33" t="str">
         <f t="shared" si="33"/>
@@ -3845,7 +3845,7 @@
         <v>28</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>98</v>
@@ -3870,15 +3870,15 @@
       </c>
       <c r="P33" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="Q33" s="31" t="str">
         <f t="shared" si="2"/>
-        <v>0001000001100101</v>
+        <v>0001000001100100</v>
       </c>
       <c r="R33" s="31" t="str">
         <f t="shared" si="3"/>
-        <v>01100101</v>
+        <v>01100100</v>
       </c>
       <c r="S33" s="31" t="str">
         <f t="shared" si="4"/>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="T33" s="31" t="str">
         <f t="shared" ref="T33:U33" si="34">BIN2HEX(R33,2)</f>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U33" s="33" t="str">
         <f t="shared" si="34"/>
@@ -3917,7 +3917,7 @@
         <v>29</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I34" s="20" t="s">
         <v>98</v>
@@ -3942,15 +3942,15 @@
       </c>
       <c r="P34" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="Q34" s="31" t="str">
         <f t="shared" si="2"/>
-        <v>0001000001100101</v>
+        <v>0001000001100100</v>
       </c>
       <c r="R34" s="31" t="str">
         <f t="shared" si="3"/>
-        <v>01100101</v>
+        <v>01100100</v>
       </c>
       <c r="S34" s="31" t="str">
         <f t="shared" si="4"/>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="T34" s="31" t="str">
         <f t="shared" ref="T34:U34" si="35">BIN2HEX(R34,2)</f>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U34" s="33" t="str">
         <f t="shared" si="35"/>
@@ -3989,7 +3989,7 @@
         <v>30</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I35" s="20" t="s">
         <v>98</v>
@@ -4014,15 +4014,15 @@
       </c>
       <c r="P35" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="Q35" s="31" t="str">
         <f t="shared" si="2"/>
-        <v>0001000001110101</v>
+        <v>0001000001110100</v>
       </c>
       <c r="R35" s="31" t="str">
         <f t="shared" si="3"/>
-        <v>01110101</v>
+        <v>01110100</v>
       </c>
       <c r="S35" s="31" t="str">
         <f t="shared" si="4"/>
@@ -4030,7 +4030,7 @@
       </c>
       <c r="T35" s="31" t="str">
         <f t="shared" ref="T35:U35" si="36">BIN2HEX(R35,2)</f>
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U35" s="33" t="str">
         <f t="shared" si="36"/>
@@ -4061,7 +4061,7 @@
         <v>31</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I36" s="20" t="s">
         <v>98</v>
@@ -4086,15 +4086,15 @@
       </c>
       <c r="P36" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="Q36" s="31" t="str">
         <f t="shared" si="2"/>
-        <v>0001000001110101</v>
+        <v>0001000001110100</v>
       </c>
       <c r="R36" s="31" t="str">
         <f t="shared" si="3"/>
-        <v>01110101</v>
+        <v>01110100</v>
       </c>
       <c r="S36" s="31" t="str">
         <f t="shared" si="4"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="T36" s="31" t="str">
         <f t="shared" ref="T36:U36" si="37">BIN2HEX(R36,2)</f>
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U36" s="33" t="str">
         <f t="shared" si="37"/>
@@ -4444,14 +4444,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="custom" allowBlank="1" sqref="O5:O16 O17:O19 O21:O30 O31:O36 O37:O40">
-      <formula1>AND(EQ(LEN(TO_TEXT(O5)),2),REGEXMATCH(TO_TEXT(O5),"[0-1]{2}"))</formula1>
-    </dataValidation>
     <dataValidation type="custom" allowBlank="1" sqref="M5:M30 M31:M36 M37:M40">
       <formula1>AND(EQ(LEN(TO_TEXT(M5)),4),REGEXMATCH(TO_TEXT(M5),"[0-1]{4}"))</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" sqref="I5:I15 I16:I27 I28:I30 I31:I36 I37:I40">
       <formula1>AND(EQ(LEN(TO_TEXT(I5)),3),REGEXMATCH(TO_TEXT(I5),"[0-1]{3}"))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" prompt="Enter 1 binary digit without a leading 0b (Ex: 0)" sqref="H5:H16">
+      <formula1>AND(EQ(LEN(TO_TEXT(H5)),1),REGEXMATCH(TO_TEXT(H5),"[0-1]{1}"))</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" sqref="O20">
       <formula1>AND(EQ(LEN(TO_TEXT(O20)),2),REGEXMATCH(TO_TEXT(O20),"[X0-1]{2}"))</formula1>
@@ -4459,8 +4459,8 @@
     <dataValidation type="custom" allowBlank="1" sqref="L20">
       <formula1>AND(EQ(LEN(TO_TEXT(L20)),1),REGEXMATCH(TO_TEXT(L20),"[0-1X]{1}"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" prompt="Enter 1 binary digit without a leading 0b (Ex: 0)" sqref="H5:H16">
-      <formula1>AND(EQ(LEN(TO_TEXT(H5)),1),REGEXMATCH(TO_TEXT(H5),"[0-1]{1}"))</formula1>
+    <dataValidation type="custom" allowBlank="1" sqref="O5:O16 O17:O19 O21:O30 O31:O36 O37:O40">
+      <formula1>AND(EQ(LEN(TO_TEXT(O5)),2),REGEXMATCH(TO_TEXT(O5),"[0-1]{2}"))</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" sqref="L17 L18 L19 H17:H18 H19:H27 H28:H30 H31:H36 H37:H40 J5:J16 J17:J27 J31:J32 J33:J36 K5:K15 K16:K27 K31:K36 L5:L16 L21:L27 L31:L36 N5:N16 N17:N30 N31:N36 N37:N40 J37:L40 J28:L30">
       <formula1>AND(EQ(LEN(TO_TEXT(H5)),1),REGEXMATCH(TO_TEXT(H5),"[0-1]{1}"))</formula1>

</xml_diff>